<commit_message>
Upload from 2015_03_21 email from Thomas Martin
</commit_message>
<xml_diff>
--- a/data/raw/FormattedBacterialMetadata.xlsx
+++ b/data/raw/FormattedBacterialMetadata.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\OneDrive\Diversity\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,11 @@
   <definedNames>
     <definedName name="_22.75___158">Sheet1!$W$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -1067,7 +1065,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1102,7 +1100,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1279,7 +1277,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1293,19 +1291,19 @@
       <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
-    <col min="14" max="14" width="46.85546875" customWidth="1"/>
-    <col min="16" max="16" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" customWidth="1"/>
+    <col min="14" max="14" width="46.83203125" customWidth="1"/>
+    <col min="16" max="16" width="22.83203125" customWidth="1"/>
     <col min="19" max="19" width="48" customWidth="1"/>
-    <col min="28" max="28" width="9" customWidth="1"/>
+    <col min="28" max="28" width="133.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1397,7 +1395,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2">
         <v>2263328039</v>
       </c>
@@ -1431,7 +1429,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3">
         <v>2513237066</v>
       </c>
@@ -1463,7 +1461,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="A4">
         <v>2524023174</v>
       </c>
@@ -1483,7 +1481,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5">
         <v>2524023082</v>
       </c>
@@ -1503,7 +1501,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6">
         <v>2522125021</v>
       </c>
@@ -1523,7 +1521,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7">
         <v>2263328040</v>
       </c>
@@ -1555,7 +1553,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8">
         <v>2264867188</v>
       </c>
@@ -1584,7 +1582,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9">
         <v>2264867157</v>
       </c>
@@ -1610,7 +1608,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10">
         <v>2524614626</v>
       </c>
@@ -1630,7 +1628,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11">
         <v>2522572196</v>
       </c>
@@ -1650,7 +1648,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30">
       <c r="A12">
         <v>2264867253</v>
       </c>
@@ -1679,7 +1677,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30">
       <c r="A13">
         <v>2236876027</v>
       </c>
@@ -1705,7 +1703,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="A14">
         <v>2264867142</v>
       </c>
@@ -1734,7 +1732,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30">
       <c r="A15">
         <v>2528768224</v>
       </c>
@@ -1757,7 +1755,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30">
       <c r="A16">
         <v>2524614624</v>
       </c>
@@ -1777,7 +1775,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29">
       <c r="A17">
         <v>2264867114</v>
       </c>
@@ -1806,7 +1804,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29">
       <c r="A18">
         <v>2527291519</v>
       </c>
@@ -1835,7 +1833,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29">
       <c r="A19">
         <v>2524614628</v>
       </c>
@@ -1855,7 +1853,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29">
       <c r="A20">
         <v>2236661001</v>
       </c>
@@ -1875,7 +1873,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29">
       <c r="A21">
         <v>2527291517</v>
       </c>
@@ -1904,7 +1902,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29">
       <c r="A22">
         <v>2236347069</v>
       </c>
@@ -1924,7 +1922,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29">
       <c r="A23">
         <v>2236347020</v>
       </c>
@@ -1953,7 +1951,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29">
       <c r="A24">
         <v>2524614796</v>
       </c>
@@ -1982,7 +1980,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29">
       <c r="A25">
         <v>2264867174</v>
       </c>
@@ -2011,7 +2009,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29">
       <c r="A26">
         <v>2265123003</v>
       </c>
@@ -2031,7 +2029,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29">
       <c r="A27">
         <v>2264867251</v>
       </c>
@@ -2060,7 +2058,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29">
       <c r="A28">
         <v>2602041625</v>
       </c>
@@ -2089,7 +2087,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29">
       <c r="A29">
         <v>2524614630</v>
       </c>
@@ -2109,7 +2107,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29">
       <c r="A30">
         <v>2236347019</v>
       </c>
@@ -2129,7 +2127,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29">
       <c r="A31">
         <v>2236347004</v>
       </c>
@@ -2158,7 +2156,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29">
       <c r="A32">
         <v>2599185278</v>
       </c>
@@ -2178,7 +2176,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28">
       <c r="A33">
         <v>2236876030</v>
       </c>
@@ -2207,7 +2205,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28">
       <c r="A34">
         <v>2228664027</v>
       </c>
@@ -2236,7 +2234,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28">
       <c r="A35">
         <v>2524614794</v>
       </c>
@@ -2265,7 +2263,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28">
       <c r="A36">
         <v>2264867242</v>
       </c>
@@ -2294,7 +2292,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28">
       <c r="A37">
         <v>2264867122</v>
       </c>
@@ -2323,7 +2321,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28">
       <c r="A38">
         <v>2236661012</v>
       </c>
@@ -2352,7 +2350,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28">
       <c r="A39">
         <v>2236347022</v>
       </c>
@@ -2381,7 +2379,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28">
       <c r="A40">
         <v>2264867105</v>
       </c>
@@ -2410,7 +2408,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28">
       <c r="A41">
         <v>2524614793</v>
       </c>
@@ -2439,7 +2437,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28">
       <c r="A42">
         <v>2264867183</v>
       </c>
@@ -2468,7 +2466,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28">
       <c r="A43">
         <v>2264867014</v>
       </c>
@@ -2488,7 +2486,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28">
       <c r="A44">
         <v>2264867198</v>
       </c>
@@ -2517,7 +2515,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28">
       <c r="A45">
         <v>2236347009</v>
       </c>
@@ -2546,7 +2544,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28">
       <c r="A46">
         <v>2558860147</v>
       </c>
@@ -2566,7 +2564,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28">
       <c r="A47">
         <v>2528768177</v>
       </c>
@@ -2589,7 +2587,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28">
       <c r="A48">
         <v>2524023063</v>
       </c>
@@ -2609,7 +2607,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28">
       <c r="A49">
         <v>2528768165</v>
       </c>
@@ -2632,7 +2630,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28">
       <c r="A50">
         <v>2524614792</v>
       </c>
@@ -2661,7 +2659,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28">
       <c r="A51">
         <v>2228664055</v>
       </c>
@@ -2690,7 +2688,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28">
       <c r="A52">
         <v>2264867176</v>
       </c>
@@ -2719,7 +2717,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28">
       <c r="A53">
         <v>2264867119</v>
       </c>
@@ -2748,7 +2746,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28">
       <c r="A54">
         <v>2264867194</v>
       </c>
@@ -2777,7 +2775,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28">
       <c r="A55">
         <v>2228664031</v>
       </c>
@@ -2806,7 +2804,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28">
       <c r="A56">
         <v>2528768172</v>
       </c>
@@ -2829,7 +2827,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28">
       <c r="A57">
         <v>2236661017</v>
       </c>
@@ -2858,7 +2856,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28">
       <c r="A58">
         <v>2236347012</v>
       </c>
@@ -2887,7 +2885,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28">
       <c r="A59">
         <v>2545555807</v>
       </c>
@@ -2907,7 +2905,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28">
       <c r="A60">
         <v>2517572139</v>
       </c>
@@ -2936,7 +2934,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28">
       <c r="A61">
         <v>2228664053</v>
       </c>
@@ -2965,7 +2963,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28">
       <c r="A62">
         <v>2264867106</v>
       </c>
@@ -2994,7 +2992,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28">
       <c r="A63">
         <v>2236661046</v>
       </c>
@@ -3014,7 +3012,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28">
       <c r="A64">
         <v>2527291521</v>
       </c>
@@ -3043,7 +3041,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:29">
       <c r="A65">
         <v>2264867214</v>
       </c>
@@ -3072,7 +3070,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29">
       <c r="A66">
         <v>2264867203</v>
       </c>
@@ -3101,7 +3099,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:29">
       <c r="A67">
         <v>2264867149</v>
       </c>
@@ -3127,7 +3125,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:29">
       <c r="A68">
         <v>2236661011</v>
       </c>
@@ -3156,7 +3154,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:29">
       <c r="A69">
         <v>2528768166</v>
       </c>
@@ -3179,7 +3177,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:29">
       <c r="A70">
         <v>2528311031</v>
       </c>
@@ -3199,7 +3197,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:29">
       <c r="A71">
         <v>2524614795</v>
       </c>
@@ -3228,7 +3226,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:29">
       <c r="A72">
         <v>2599185281</v>
       </c>
@@ -3248,7 +3246,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:29">
       <c r="A73">
         <v>2524614788</v>
       </c>
@@ -3277,7 +3275,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:29">
       <c r="A74">
         <v>2505119051</v>
       </c>
@@ -3309,7 +3307,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:29">
       <c r="A75">
         <v>2228664029</v>
       </c>
@@ -3338,7 +3336,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:29">
       <c r="A76">
         <v>2264867144</v>
       </c>
@@ -3367,7 +3365,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:29">
       <c r="A77">
         <v>2228664026</v>
       </c>
@@ -3393,7 +3391,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:29">
       <c r="A78">
         <v>2558860156</v>
       </c>
@@ -3413,7 +3411,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:29">
       <c r="A79">
         <v>2517572140</v>
       </c>
@@ -3442,7 +3440,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:29">
       <c r="A80">
         <v>2264867058</v>
       </c>
@@ -3471,7 +3469,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28">
       <c r="A81">
         <v>2599185269</v>
       </c>
@@ -3491,7 +3489,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28">
       <c r="A82">
         <v>2523533602</v>
       </c>
@@ -3511,7 +3509,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28">
       <c r="A83">
         <v>2599185284</v>
       </c>
@@ -3531,7 +3529,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28">
       <c r="A84">
         <v>2518285600</v>
       </c>
@@ -3560,7 +3558,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28">
       <c r="A85">
         <v>2264867201</v>
       </c>
@@ -3589,7 +3587,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28">
       <c r="A86">
         <v>2528311066</v>
       </c>
@@ -3612,7 +3610,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28">
       <c r="A87">
         <v>2524023083</v>
       </c>
@@ -3632,7 +3630,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:28">
       <c r="A88">
         <v>2228664032</v>
       </c>
@@ -3661,7 +3659,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:28">
       <c r="A89">
         <v>2527291516</v>
       </c>
@@ -3690,7 +3688,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:28">
       <c r="A90">
         <v>2264867152</v>
       </c>
@@ -3716,7 +3714,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:28">
       <c r="A91">
         <v>2264867009</v>
       </c>
@@ -3736,7 +3734,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:28">
       <c r="A92">
         <v>2228664028</v>
       </c>
@@ -3765,7 +3763,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:28">
       <c r="A93">
         <v>2599185275</v>
       </c>
@@ -3785,7 +3783,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:28">
       <c r="A94">
         <v>2522572187</v>
       </c>
@@ -3805,7 +3803,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:28">
       <c r="A95">
         <v>2599185282</v>
       </c>
@@ -3825,7 +3823,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28">
       <c r="A96">
         <v>2264867180</v>
       </c>
@@ -3854,7 +3852,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:28">
       <c r="A97">
         <v>2264867011</v>
       </c>
@@ -3874,7 +3872,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28">
       <c r="A98">
         <v>2228664051</v>
       </c>
@@ -3903,7 +3901,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28">
       <c r="A99">
         <v>2264867111</v>
       </c>
@@ -3932,7 +3930,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28">
       <c r="A100">
         <v>2264867167</v>
       </c>
@@ -3961,7 +3959,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28">
       <c r="A101">
         <v>2264867013</v>
       </c>
@@ -3981,7 +3979,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28">
       <c r="A102">
         <v>2523231004</v>
       </c>
@@ -4001,7 +3999,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28">
       <c r="A103">
         <v>2264867108</v>
       </c>
@@ -4030,7 +4028,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28">
       <c r="A104">
         <v>2524023080</v>
       </c>
@@ -4050,7 +4048,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28">
       <c r="A105">
         <v>2236661005</v>
       </c>
@@ -4070,7 +4068,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28">
       <c r="A106">
         <v>2236347013</v>
       </c>
@@ -4099,7 +4097,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:28">
       <c r="A107">
         <v>2236876032</v>
       </c>
@@ -4125,7 +4123,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:28">
       <c r="A108">
         <v>2558860153</v>
       </c>
@@ -4145,7 +4143,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:28">
       <c r="A109">
         <v>2524614791</v>
       </c>
@@ -4174,7 +4172,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:28">
       <c r="A110">
         <v>2599185277</v>
       </c>
@@ -4194,7 +4192,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:28">
       <c r="A111">
         <v>2527291527</v>
       </c>
@@ -4223,7 +4221,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28">
       <c r="A112">
         <v>2264867165</v>
       </c>
@@ -4252,7 +4250,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="113" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:28">
       <c r="A113">
         <v>2264867099</v>
       </c>
@@ -4281,7 +4279,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="114" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:28">
       <c r="A114">
         <v>2524023175</v>
       </c>
@@ -4301,7 +4299,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="115" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:28">
       <c r="A115">
         <v>2599185280</v>
       </c>
@@ -4321,7 +4319,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="116" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:28">
       <c r="A116">
         <v>2236347005</v>
       </c>
@@ -4350,7 +4348,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="117" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:28">
       <c r="A117">
         <v>2264867206</v>
       </c>
@@ -4376,7 +4374,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="118" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:28">
       <c r="A118">
         <v>2228664052</v>
       </c>
@@ -4405,7 +4403,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="119" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:28">
       <c r="A119">
         <v>2264867005</v>
       </c>
@@ -4434,7 +4432,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="120" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:28">
       <c r="A120">
         <v>2264867110</v>
       </c>
@@ -4463,7 +4461,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="121" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:28">
       <c r="A121">
         <v>2264867182</v>
       </c>
@@ -4492,7 +4490,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="122" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:28">
       <c r="A122">
         <v>2264867054</v>
       </c>
@@ -4521,7 +4519,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="123" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:28">
       <c r="A123">
         <v>2599185273</v>
       </c>
@@ -4541,7 +4539,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="124" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:28">
       <c r="A124">
         <v>2236347016</v>
       </c>
@@ -4570,7 +4568,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="125" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:28">
       <c r="A125">
         <v>2524614629</v>
       </c>
@@ -4590,7 +4588,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="126" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:28">
       <c r="A126">
         <v>2264867107</v>
       </c>
@@ -4619,7 +4617,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="127" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:28">
       <c r="A127">
         <v>2264867173</v>
       </c>
@@ -4648,7 +4646,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="128" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:28">
       <c r="A128">
         <v>2264867254</v>
       </c>
@@ -4677,7 +4675,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="129" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:28">
       <c r="A129">
         <v>2264867109</v>
       </c>
@@ -4706,7 +4704,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="130" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:28">
       <c r="A130">
         <v>2524023235</v>
       </c>
@@ -4726,7 +4724,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="131" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:28">
       <c r="A131">
         <v>2264867016</v>
       </c>
@@ -4746,7 +4744,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="132" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:28">
       <c r="A132">
         <v>2524614627</v>
       </c>
@@ -4766,7 +4764,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="133" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:28">
       <c r="A133">
         <v>2264867240</v>
       </c>
@@ -4792,7 +4790,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="134" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:28">
       <c r="A134">
         <v>2558860150</v>
       </c>
@@ -4812,7 +4810,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="135" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:28">
       <c r="A135">
         <v>2558860149</v>
       </c>
@@ -4832,7 +4830,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="136" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:28">
       <c r="A136">
         <v>2522572185</v>
       </c>
@@ -4852,7 +4850,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="137" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:28">
       <c r="A137">
         <v>2599185279</v>
       </c>
@@ -4872,7 +4870,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="138" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:28">
       <c r="A138">
         <v>2505679121</v>
       </c>
@@ -4892,7 +4890,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="139" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:28">
       <c r="A139">
         <v>2528768162</v>
       </c>
@@ -4915,7 +4913,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="140" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:28">
       <c r="A140">
         <v>2519103005</v>
       </c>
@@ -4935,7 +4933,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="141" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:28">
       <c r="A141">
         <v>2264867200</v>
       </c>
@@ -4964,7 +4962,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="142" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:28">
       <c r="A142">
         <v>2558860164</v>
       </c>
@@ -4987,7 +4985,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="143" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:28">
       <c r="A143">
         <v>2264867148</v>
       </c>
@@ -5016,7 +5014,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="144" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:28">
       <c r="A144">
         <v>2264867195</v>
       </c>
@@ -5045,7 +5043,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="145" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:29">
       <c r="A145">
         <v>2236661009</v>
       </c>
@@ -5065,7 +5063,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="146" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:29">
       <c r="A146">
         <v>2264867186</v>
       </c>
@@ -5094,7 +5092,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="147" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:29">
       <c r="A147">
         <v>2228664034</v>
       </c>
@@ -5123,7 +5121,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="148" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:29">
       <c r="A148">
         <v>2236876028</v>
       </c>
@@ -5143,7 +5141,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="149" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:29">
       <c r="A149">
         <v>2264867184</v>
       </c>
@@ -5172,7 +5170,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="150" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:29">
       <c r="A150">
         <v>2599185258</v>
       </c>
@@ -5192,7 +5190,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="151" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:29">
       <c r="A151">
         <v>2264265094</v>
       </c>
@@ -5218,7 +5216,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="152" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:29">
       <c r="A152">
         <v>2524023178</v>
       </c>
@@ -5238,7 +5236,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="153" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:29">
       <c r="A153">
         <v>2524023081</v>
       </c>
@@ -5258,7 +5256,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="154" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:29">
       <c r="A154">
         <v>2228664038</v>
       </c>
@@ -5287,7 +5285,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="155" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:29">
       <c r="A155">
         <v>2236876029</v>
       </c>
@@ -5313,7 +5311,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="156" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:29">
       <c r="A156">
         <v>2524023066</v>
       </c>
@@ -5333,7 +5331,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="157" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:29">
       <c r="A157">
         <v>2527291520</v>
       </c>
@@ -5362,7 +5360,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="158" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:29">
       <c r="A158">
         <v>2524023079</v>
       </c>
@@ -5382,7 +5380,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="159" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:29">
       <c r="A159">
         <v>2264867241</v>
       </c>
@@ -5414,7 +5412,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="160" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:29">
       <c r="A160">
         <v>2263328036</v>
       </c>
@@ -5446,7 +5444,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="161" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:29">
       <c r="A161">
         <v>2228664030</v>
       </c>
@@ -5472,7 +5470,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="162" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:29">
       <c r="A162">
         <v>2236661015</v>
       </c>
@@ -5501,7 +5499,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="163" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:29">
       <c r="A163">
         <v>2527291515</v>
       </c>
@@ -5530,7 +5528,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="164" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:29">
       <c r="A164">
         <v>2228664056</v>
       </c>
@@ -5559,7 +5557,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="165" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:29">
       <c r="A165">
         <v>2264867189</v>
       </c>
@@ -5588,7 +5586,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="166" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:29">
       <c r="A166">
         <v>2236347014</v>
       </c>
@@ -5617,7 +5615,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="167" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:29">
       <c r="A167">
         <v>2517572141</v>
       </c>
@@ -5646,7 +5644,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="168" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:29">
       <c r="A168">
         <v>2264867177</v>
       </c>
@@ -5675,7 +5673,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="169" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:29">
       <c r="A169">
         <v>2264867190</v>
       </c>
@@ -5704,7 +5702,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="170" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:29">
       <c r="A170">
         <v>2264867089</v>
       </c>
@@ -5733,7 +5731,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="171" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:29">
       <c r="A171">
         <v>2505119050</v>
       </c>
@@ -5765,7 +5763,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="172" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:29">
       <c r="A172">
         <v>2599185294</v>
       </c>
@@ -5785,7 +5783,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="173" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:29">
       <c r="A173">
         <v>2264867045</v>
       </c>
@@ -5805,7 +5803,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="174" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:29">
       <c r="A174">
         <v>2228664039</v>
       </c>
@@ -5834,7 +5832,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="175" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:29">
       <c r="A175">
         <v>2528311067</v>
       </c>
@@ -5857,7 +5855,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="176" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:29">
       <c r="A176">
         <v>2264867158</v>
       </c>
@@ -5886,7 +5884,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="177" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:28">
       <c r="A177">
         <v>2599185293</v>
       </c>
@@ -5906,7 +5904,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="178" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:28">
       <c r="A178">
         <v>2264867051</v>
       </c>
@@ -5926,7 +5924,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="179" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:28">
       <c r="A179">
         <v>2264867150</v>
       </c>
@@ -5952,7 +5950,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="180" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:28">
       <c r="A180">
         <v>2517572142</v>
       </c>
@@ -5981,7 +5979,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="181" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:28">
       <c r="A181">
         <v>2236347008</v>
       </c>
@@ -6010,7 +6008,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="182" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:28">
       <c r="A182">
         <v>2228664040</v>
       </c>
@@ -6039,7 +6037,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="183" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:28">
       <c r="A183">
         <v>2558860155</v>
       </c>
@@ -6059,7 +6057,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="184" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:28">
       <c r="A184">
         <v>2524023064</v>
       </c>
@@ -6079,7 +6077,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="185" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:28">
       <c r="A185">
         <v>2264867162</v>
       </c>
@@ -6105,7 +6103,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="186" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:28">
       <c r="A186">
         <v>2264867202</v>
       </c>
@@ -6134,7 +6132,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="187" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:28">
       <c r="A187">
         <v>2524023172</v>
       </c>
@@ -6154,7 +6152,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="188" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:28">
       <c r="A188">
         <v>2264867012</v>
       </c>
@@ -6174,7 +6172,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="189" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:28">
       <c r="A189">
         <v>2599185286</v>
       </c>
@@ -6194,7 +6192,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="190" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:28">
       <c r="A190">
         <v>2264867151</v>
       </c>
@@ -6220,7 +6218,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="191" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:28">
       <c r="A191">
         <v>2264867196</v>
       </c>
@@ -6249,7 +6247,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="192" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:28">
       <c r="A192">
         <v>2264867098</v>
       </c>
@@ -6278,7 +6276,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="193" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:28">
       <c r="A193">
         <v>2528311029</v>
       </c>
@@ -6298,7 +6296,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="194" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:28">
       <c r="A194">
         <v>2519899769</v>
       </c>
@@ -6318,7 +6316,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="195" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:28">
       <c r="A195">
         <v>2264867010</v>
       </c>
@@ -6338,7 +6336,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="196" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:28">
       <c r="A196">
         <v>2264867004</v>
       </c>
@@ -6367,7 +6365,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="197" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:28">
       <c r="A197">
         <v>2264867112</v>
       </c>
@@ -6396,7 +6394,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="198" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:28">
       <c r="A198">
         <v>2264867115</v>
       </c>
@@ -6425,7 +6423,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="199" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:28">
       <c r="A199">
         <v>2264867175</v>
       </c>
@@ -6454,7 +6452,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="200" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:28">
       <c r="A200">
         <v>2264867209</v>
       </c>
@@ -6480,7 +6478,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="201" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:28">
       <c r="A201">
         <v>2264867187</v>
       </c>
@@ -6509,7 +6507,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="202" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:28">
       <c r="A202">
         <v>2518285508</v>
       </c>
@@ -6529,7 +6527,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="203" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:28">
       <c r="A203">
         <v>2558860152</v>
       </c>
@@ -6549,7 +6547,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="204" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:28">
       <c r="A204">
         <v>2524023189</v>
       </c>
@@ -6569,7 +6567,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="205" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:28">
       <c r="A205">
         <v>2523533603</v>
       </c>
@@ -6589,7 +6587,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="206" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:28">
       <c r="A206">
         <v>2236661010</v>
       </c>
@@ -6615,7 +6613,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="207" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:28">
       <c r="A207">
         <v>2236347002</v>
       </c>
@@ -6644,7 +6642,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="208" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:28">
       <c r="A208">
         <v>2558860154</v>
       </c>
@@ -6664,7 +6662,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="209" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:29">
       <c r="A209">
         <v>2524614790</v>
       </c>
@@ -6693,7 +6691,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="210" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:29">
       <c r="A210">
         <v>2545555832</v>
       </c>
@@ -6713,7 +6711,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="211" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:29">
       <c r="A211">
         <v>2524614625</v>
       </c>
@@ -6733,7 +6731,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="212" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:29">
       <c r="A212">
         <v>2264867079</v>
       </c>
@@ -6762,7 +6760,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="213" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:29">
       <c r="A213">
         <v>2228664044</v>
       </c>
@@ -6791,7 +6789,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="214" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:29">
       <c r="A214">
         <v>2602042074</v>
       </c>
@@ -6811,7 +6809,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="215" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:29">
       <c r="A215">
         <v>2264867123</v>
       </c>
@@ -6840,7 +6838,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="216" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:29">
       <c r="A216">
         <v>2264867141</v>
       </c>
@@ -6866,7 +6864,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="217" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:29">
       <c r="A217">
         <v>2541046968</v>
       </c>
@@ -6886,7 +6884,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="218" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:29">
       <c r="A218">
         <v>2524023176</v>
       </c>
@@ -6906,7 +6904,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="219" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:29">
       <c r="A219">
         <v>2505119052</v>
       </c>
@@ -6938,7 +6936,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="220" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:29">
       <c r="A220">
         <v>2264867181</v>
       </c>
@@ -6967,7 +6965,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="221" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:29">
       <c r="A221">
         <v>2264867168</v>
       </c>
@@ -6996,7 +6994,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="222" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:29">
       <c r="A222">
         <v>2236661004</v>
       </c>
@@ -7016,7 +7014,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="223" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:29">
       <c r="A223">
         <v>2264867117</v>
       </c>
@@ -7045,7 +7043,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="224" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:29">
       <c r="A224">
         <v>2599185276</v>
       </c>
@@ -7065,7 +7063,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="225" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:28">
       <c r="A225">
         <v>2236661007</v>
       </c>
@@ -7085,7 +7083,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="226" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:28">
       <c r="A226">
         <v>2264867243</v>
       </c>
@@ -7116,6 +7114,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>